<commit_message>
Adding data for validation plotting inputs.
Revised short spreadsheet output to eliminate blank line ... pyrograph processing did not like the blank line.
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/ValidationColumnMappings.xlsx
+++ b/cfast/trunk/Validation/ValidationColumnMappings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="122">
   <si>
     <t>CFAST Time</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>x 0.001</t>
+  </si>
+  <si>
+    <t>VTT C2</t>
   </si>
 </sst>
 </file>
@@ -723,7 +726,7 @@
   <dimension ref="A1:BI15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AG7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15"/>
@@ -812,7 +815,7 @@
     </row>
     <row r="5" spans="1:61">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -1388,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15"/>
@@ -1474,7 +1477,7 @@
     </row>
     <row r="5" spans="1:61">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>

</xml_diff>